<commit_message>
add an sample in 202108101638
</commit_message>
<xml_diff>
--- a/statistics/data/test0.xlsx
+++ b/statistics/data/test0.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView windowWidth="21600" windowHeight="10730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="491">
   <si>
     <t>序号</t>
   </si>
@@ -958,10 +957,130 @@
     <t>2030031096</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>2021/3/4 18:59:30</t>
+    <t>54</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:00:37</t>
+  </si>
+  <si>
+    <t>王艺霖</t>
+  </si>
+  <si>
+    <t>2030001093</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:02:40</t>
+  </si>
+  <si>
+    <t>204秒</t>
+  </si>
+  <si>
+    <t>李子君</t>
+  </si>
+  <si>
+    <t>1930013018</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:03:47</t>
+  </si>
+  <si>
+    <t>169秒</t>
+  </si>
+  <si>
+    <t>14.27.1.119(广东-广州)</t>
+  </si>
+  <si>
+    <t>刘熠清</t>
+  </si>
+  <si>
+    <t>1830024171</t>
+  </si>
+  <si>
+    <t>秋江夜泊 周一 18:10-19:10┋春晓吟 周四 18:10-19:10</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:14:35</t>
+  </si>
+  <si>
+    <t>112.97.84.156(广东-深圳)</t>
+  </si>
+  <si>
+    <t>刘奕含</t>
+  </si>
+  <si>
+    <t>2030031126</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:18:10</t>
+  </si>
+  <si>
+    <t>71秒</t>
+  </si>
+  <si>
+    <t>117.136.33.85(广东-东莞)</t>
+  </si>
+  <si>
+    <t>东蕊</t>
+  </si>
+  <si>
+    <t>1830025019</t>
+  </si>
+  <si>
+    <t>春晓吟 周四 18:10-19:10</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:20:45</t>
+  </si>
+  <si>
+    <t>136秒</t>
+  </si>
+  <si>
+    <t>庞澍</t>
+  </si>
+  <si>
+    <t>1930031137</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:21:20</t>
+  </si>
+  <si>
+    <t>122秒</t>
+  </si>
+  <si>
+    <t>117.136.41.30(广东-佛山)</t>
+  </si>
+  <si>
+    <t>蔺殊嘉</t>
+  </si>
+  <si>
+    <t>1930005030</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:23:59</t>
+  </si>
+  <si>
+    <t>48秒</t>
   </si>
   <si>
     <t>117.136.32.76(广东-深圳)</t>
@@ -970,337 +1089,211 @@
     <t>李嵋</t>
   </si>
   <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:26:49</t>
+  </si>
+  <si>
+    <t>30秒</t>
+  </si>
+  <si>
+    <t>117.136.32.79(广东-深圳)</t>
+  </si>
+  <si>
+    <t>李佳璇</t>
+  </si>
+  <si>
+    <t>1830025056</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:33:51</t>
+  </si>
+  <si>
+    <t>68秒</t>
+  </si>
+  <si>
+    <t>117.136.79.79(广东-珠海)</t>
+  </si>
+  <si>
+    <t>杜嘉琦</t>
+  </si>
+  <si>
+    <t>1830026022</t>
+  </si>
+  <si>
+    <t>湘江怨 周三 19:30-20:30┋春晓吟 周四 18:10-19:10</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:37:08</t>
+  </si>
+  <si>
+    <t>84秒</t>
+  </si>
+  <si>
+    <t>112.96.137.175(广东-广州)</t>
+  </si>
+  <si>
+    <t>冯意如</t>
+  </si>
+  <si>
+    <t>1930006040</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:53:39</t>
+  </si>
+  <si>
+    <t>280秒</t>
+  </si>
+  <si>
+    <t>14.27.32.74(广东-广州)</t>
+  </si>
+  <si>
+    <t>韦安淇</t>
+  </si>
+  <si>
+    <t>1830024269</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:55:25</t>
+  </si>
+  <si>
+    <t>117.136.32.69(广东-深圳)</t>
+  </si>
+  <si>
+    <t>赵舜雨</t>
+  </si>
+  <si>
+    <t>2030001132</t>
+  </si>
+  <si>
+    <t>杨官林</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:58:08</t>
+  </si>
+  <si>
+    <t>14.25.149.138(广东-广州)</t>
+  </si>
+  <si>
+    <t>张诗琪</t>
+  </si>
+  <si>
+    <t>1930025122</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>2021/3/4 19:58:40</t>
+  </si>
+  <si>
+    <t>82秒</t>
+  </si>
+  <si>
+    <t>112.96.106.87(广东-广州)</t>
+  </si>
+  <si>
+    <t>李元昊</t>
+  </si>
+  <si>
+    <t>1830026070</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>2021/3/4 20:05:32</t>
+  </si>
+  <si>
+    <t>209秒</t>
+  </si>
+  <si>
+    <t>223.104.60.133(广东-广州)</t>
+  </si>
+  <si>
+    <t>朱烨</t>
+  </si>
+  <si>
+    <t>1830001131</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>2021/3/4 20:07:25</t>
+  </si>
+  <si>
+    <t>130秒</t>
+  </si>
+  <si>
+    <t>117.136.31.46(广东-广州)</t>
+  </si>
+  <si>
+    <t>徐睿</t>
+  </si>
+  <si>
+    <t>1930004039</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>2021/3/4 20:13:28</t>
+  </si>
+  <si>
+    <t>钟偲睿</t>
+  </si>
+  <si>
+    <t>2030006268</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>2021/3/4 20:25:49</t>
+  </si>
+  <si>
+    <t>51秒</t>
+  </si>
+  <si>
+    <t>刘雯钰</t>
+  </si>
+  <si>
+    <t>2030006119</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>2021/3/4 20:42:44</t>
+  </si>
+  <si>
+    <t>117.136.12.125(广东-佛山)</t>
+  </si>
+  <si>
+    <t>王淳羚</t>
+  </si>
+  <si>
+    <t>1930031165</t>
+  </si>
+  <si>
     <t>太古引 周一 19:30-20:30┋凤求凰 周二 18:10-19:10</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:00:37</t>
-  </si>
-  <si>
-    <t>王艺霖</t>
-  </si>
-  <si>
-    <t>2030001093</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:02:40</t>
-  </si>
-  <si>
-    <t>204秒</t>
-  </si>
-  <si>
-    <t>李子君</t>
-  </si>
-  <si>
-    <t>1930013018</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:03:47</t>
-  </si>
-  <si>
-    <t>169秒</t>
-  </si>
-  <si>
-    <t>14.27.1.119(广东-广州)</t>
-  </si>
-  <si>
-    <t>刘熠清</t>
-  </si>
-  <si>
-    <t>1830024171</t>
-  </si>
-  <si>
-    <t>秋江夜泊 周一 18:10-19:10┋春晓吟 周四 18:10-19:10</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:14:35</t>
-  </si>
-  <si>
-    <t>112.97.84.156(广东-深圳)</t>
-  </si>
-  <si>
-    <t>刘奕含</t>
-  </si>
-  <si>
-    <t>2030031126</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:18:10</t>
-  </si>
-  <si>
-    <t>71秒</t>
-  </si>
-  <si>
-    <t>117.136.33.85(广东-东莞)</t>
-  </si>
-  <si>
-    <t>东蕊</t>
-  </si>
-  <si>
-    <t>1830025019</t>
-  </si>
-  <si>
-    <t>春晓吟 周四 18:10-19:10</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:20:45</t>
-  </si>
-  <si>
-    <t>136秒</t>
-  </si>
-  <si>
-    <t>庞澍</t>
-  </si>
-  <si>
-    <t>1930031137</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:21:20</t>
-  </si>
-  <si>
-    <t>122秒</t>
-  </si>
-  <si>
-    <t>117.136.41.30(广东-佛山)</t>
-  </si>
-  <si>
-    <t>蔺殊嘉</t>
-  </si>
-  <si>
-    <t>1930005030</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:23:59</t>
-  </si>
-  <si>
-    <t>48秒</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:26:49</t>
-  </si>
-  <si>
-    <t>30秒</t>
-  </si>
-  <si>
-    <t>117.136.32.79(广东-深圳)</t>
-  </si>
-  <si>
-    <t>李佳璇</t>
-  </si>
-  <si>
-    <t>1830025056</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:33:51</t>
-  </si>
-  <si>
-    <t>68秒</t>
-  </si>
-  <si>
-    <t>117.136.79.79(广东-珠海)</t>
-  </si>
-  <si>
-    <t>杜嘉琦</t>
-  </si>
-  <si>
-    <t>1830026022</t>
-  </si>
-  <si>
-    <t>湘江怨 周三 19:30-20:30┋春晓吟 周四 18:10-19:10</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:37:08</t>
-  </si>
-  <si>
-    <t>84秒</t>
-  </si>
-  <si>
-    <t>112.96.137.175(广东-广州)</t>
-  </si>
-  <si>
-    <t>冯意如</t>
-  </si>
-  <si>
-    <t>1930006040</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:53:39</t>
-  </si>
-  <si>
-    <t>280秒</t>
-  </si>
-  <si>
-    <t>14.27.32.74(广东-广州)</t>
-  </si>
-  <si>
-    <t>韦安淇</t>
-  </si>
-  <si>
-    <t>1830024269</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:55:25</t>
-  </si>
-  <si>
-    <t>117.136.32.69(广东-深圳)</t>
-  </si>
-  <si>
-    <t>赵舜雨</t>
-  </si>
-  <si>
-    <t>2030001132</t>
-  </si>
-  <si>
-    <t>杨官林</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:58:08</t>
-  </si>
-  <si>
-    <t>14.25.149.138(广东-广州)</t>
-  </si>
-  <si>
-    <t>张诗琪</t>
-  </si>
-  <si>
-    <t>1930025122</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>2021/3/4 19:58:40</t>
-  </si>
-  <si>
-    <t>82秒</t>
-  </si>
-  <si>
-    <t>112.96.106.87(广东-广州)</t>
-  </si>
-  <si>
-    <t>李元昊</t>
-  </si>
-  <si>
-    <t>1830026070</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>2021/3/4 20:05:32</t>
-  </si>
-  <si>
-    <t>209秒</t>
-  </si>
-  <si>
-    <t>223.104.60.133(广东-广州)</t>
-  </si>
-  <si>
-    <t>朱烨</t>
-  </si>
-  <si>
-    <t>1830001131</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>2021/3/4 20:07:25</t>
-  </si>
-  <si>
-    <t>130秒</t>
-  </si>
-  <si>
-    <t>117.136.31.46(广东-广州)</t>
-  </si>
-  <si>
-    <t>徐睿</t>
-  </si>
-  <si>
-    <t>1930004039</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>2021/3/4 20:13:28</t>
-  </si>
-  <si>
-    <t>钟偲睿</t>
-  </si>
-  <si>
-    <t>2030006268</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>2021/3/4 20:25:49</t>
-  </si>
-  <si>
-    <t>51秒</t>
-  </si>
-  <si>
-    <t>刘雯钰</t>
-  </si>
-  <si>
-    <t>2030006119</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>2021/3/4 20:42:44</t>
-  </si>
-  <si>
-    <t>117.136.12.125(广东-佛山)</t>
-  </si>
-  <si>
-    <t>王淳羚</t>
-  </si>
-  <si>
-    <t>1930031165</t>
   </si>
   <si>
     <t>74</t>
@@ -1502,22 +1495,365 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1525,111 +1861,326 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
+  <cellStyleXfs count="55">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="51"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Percent" xfId="15"/>
-    <cellStyle name="Currency" xfId="16"/>
-    <cellStyle name="Currency [0]" xfId="17"/>
-    <cellStyle name="Comma" xfId="18"/>
-    <cellStyle name="Comma [0]" xfId="19"/>
+  <cellStyles count="55">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="Currency" xfId="12"/>
+    <cellStyle name="已访问的超链接" xfId="13" builtinId="9"/>
+    <cellStyle name="注释" xfId="14" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
+    <cellStyle name="标题" xfId="18" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
+    <cellStyle name="输出" xfId="25" builtinId="21"/>
+    <cellStyle name="计算" xfId="26" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
+    <cellStyle name="Currency [0]" xfId="28"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="29" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="30" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="31" builtinId="24"/>
+    <cellStyle name="汇总" xfId="32" builtinId="25"/>
+    <cellStyle name="好" xfId="33" builtinId="26"/>
+    <cellStyle name="适中" xfId="34" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="36" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="37" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="38" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="39" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="40" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="41" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="42" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="43" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="44" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="45" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="46" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="47" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="48" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="49" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="50" builtinId="52"/>
+    <cellStyle name="Normal" xfId="51"/>
+    <cellStyle name="Percent" xfId="52"/>
+    <cellStyle name="Comma [0]" xfId="53"/>
+    <cellStyle name="Comma" xfId="54"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1947,38 +2498,40 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A54" sqref="$A54:$XFD54"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="4.14285714285714" customWidth="1"/>
-    <col min="2" max="2" width="16.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="4.14545454545455" customWidth="1"/>
+    <col min="2" max="2" width="16.1454545454545" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="4.14285714285714" customWidth="1"/>
+    <col min="4" max="4" width="4.14545454545455" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="21.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="25.5714285714286" customWidth="1"/>
-    <col min="8" max="8" width="5.57142857142857" customWidth="1"/>
-    <col min="9" max="9" width="11.2857142857143" customWidth="1"/>
-    <col min="10" max="10" width="9.85714285714286" customWidth="1"/>
-    <col min="11" max="11" width="22.7142857142857" customWidth="1"/>
-    <col min="12" max="13" width="59.5714285714286" customWidth="1"/>
-    <col min="14" max="14" width="22.7142857142857" customWidth="1"/>
-    <col min="15" max="15" width="41.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="21.4272727272727" customWidth="1"/>
+    <col min="7" max="7" width="25.5727272727273" customWidth="1"/>
+    <col min="8" max="8" width="5.57272727272727" customWidth="1"/>
+    <col min="9" max="9" width="11.2818181818182" customWidth="1"/>
+    <col min="10" max="10" width="9.85454545454546" customWidth="1"/>
+    <col min="11" max="11" width="22.7181818181818" customWidth="1"/>
+    <col min="12" max="13" width="59.5727272727273" customWidth="1"/>
+    <col min="14" max="14" width="22.7181818181818" customWidth="1"/>
+    <col min="15" max="15" width="41.5727272727273" customWidth="1"/>
     <col min="16" max="16" width="61" customWidth="1"/>
-    <col min="17" max="17" width="31.7142857142857" customWidth="1"/>
-    <col min="18" max="18" width="11.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="31.7181818181818" customWidth="1"/>
+    <col min="18" max="18" width="11.2818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="12.75">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2034,7 +2587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12.75">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2090,7 +2643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12.75">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2146,7 +2699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12.75">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2202,7 +2755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.75">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2258,7 +2811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12.75">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2314,7 +2867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12.75">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2370,7 +2923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12.75">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2426,7 +2979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="12.75">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -2482,7 +3035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12.75">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -2538,7 +3091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12.75">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2594,7 +3147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12.75">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -2650,7 +3203,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.75">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -2706,7 +3259,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12.75">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -2762,7 +3315,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12.75">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -2818,7 +3371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12.75">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -2874,7 +3427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12.75">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -2930,7 +3483,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12.75">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2986,7 +3539,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="12.75">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -3042,7 +3595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="12.75">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -3098,7 +3651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="12.75">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -3154,7 +3707,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="12.75">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>139</v>
       </c>
@@ -3210,7 +3763,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12.75">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>141</v>
       </c>
@@ -3266,7 +3819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12.75">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -3322,7 +3875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12.75">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3378,7 +3931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="12.75">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -3434,7 +3987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="12.75">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>162</v>
       </c>
@@ -3490,7 +4043,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="12.75">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -3546,7 +4099,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="12.75">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>173</v>
       </c>
@@ -3602,7 +4155,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="12.75">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -3658,7 +4211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12.75">
+    <row r="31" spans="1:18">
       <c r="A31" t="s">
         <v>186</v>
       </c>
@@ -3714,7 +4267,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="12.75">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -3770,7 +4323,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="12.75">
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
         <v>194</v>
       </c>
@@ -3826,7 +4379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="12.75">
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
         <v>200</v>
       </c>
@@ -3882,7 +4435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="12.75">
+    <row r="35" spans="1:18">
       <c r="A35" t="s">
         <v>205</v>
       </c>
@@ -3938,7 +4491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="12.75">
+    <row r="36" spans="1:18">
       <c r="A36" t="s">
         <v>210</v>
       </c>
@@ -3994,7 +4547,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="12.75">
+    <row r="37" spans="1:18">
       <c r="A37" t="s">
         <v>214</v>
       </c>
@@ -4050,7 +4603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="12.75">
+    <row r="38" spans="1:18">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -4106,7 +4659,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12.75">
+    <row r="39" spans="1:18">
       <c r="A39" t="s">
         <v>228</v>
       </c>
@@ -4162,7 +4715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="12.75">
+    <row r="40" spans="1:18">
       <c r="A40" t="s">
         <v>234</v>
       </c>
@@ -4218,7 +4771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="12.75">
+    <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>238</v>
       </c>
@@ -4274,7 +4827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="12.75">
+    <row r="42" spans="1:18">
       <c r="A42" t="s">
         <v>243</v>
       </c>
@@ -4330,7 +4883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="12.75">
+    <row r="43" spans="1:18">
       <c r="A43" t="s">
         <v>249</v>
       </c>
@@ -4386,7 +4939,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="12.75">
+    <row r="44" spans="1:18">
       <c r="A44" t="s">
         <v>255</v>
       </c>
@@ -4442,7 +4995,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="12.75">
+    <row r="45" spans="1:18">
       <c r="A45" t="s">
         <v>262</v>
       </c>
@@ -4498,7 +5051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="12.75">
+    <row r="46" spans="1:18">
       <c r="A46" t="s">
         <v>267</v>
       </c>
@@ -4554,7 +5107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="12.75">
+    <row r="47" spans="1:18">
       <c r="A47" t="s">
         <v>272</v>
       </c>
@@ -4610,7 +5163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="12.75">
+    <row r="48" spans="1:18">
       <c r="A48" t="s">
         <v>278</v>
       </c>
@@ -4666,7 +5219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="12.75">
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>284</v>
       </c>
@@ -4722,7 +5275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="12.75">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>293</v>
       </c>
@@ -4778,7 +5331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="12.75">
+    <row r="51" spans="1:18">
       <c r="A51" t="s">
         <v>297</v>
       </c>
@@ -4834,7 +5387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="12.75">
+    <row r="52" spans="1:18">
       <c r="A52" t="s">
         <v>303</v>
       </c>
@@ -4890,7 +5443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="12.75">
+    <row r="53" spans="1:18">
       <c r="A53" t="s">
         <v>308</v>
       </c>
@@ -4946,7 +5499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="12.75">
+    <row r="54" spans="1:18">
       <c r="A54" t="s">
         <v>313</v>
       </c>
@@ -4954,7 +5507,7 @@
         <v>314</v>
       </c>
       <c r="C54" t="s">
-        <v>295</v>
+        <v>191</v>
       </c>
       <c r="D54" t="s">
         <v>16</v>
@@ -4963,54 +5516,54 @@
         <v>17</v>
       </c>
       <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" t="s">
         <v>315</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
+        <v>37</v>
+      </c>
+      <c r="I54" t="s">
         <v>316</v>
       </c>
-      <c r="H54" t="s">
-        <v>209</v>
-      </c>
-      <c r="I54" t="s">
-        <v>23</v>
-      </c>
       <c r="J54" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="K54" t="s">
         <v>23</v>
       </c>
       <c r="L54" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="M54" t="s">
+        <v>23</v>
+      </c>
+      <c r="N54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>25</v>
+      </c>
+      <c r="R54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
         <v>317</v>
       </c>
-      <c r="N54" t="s">
-        <v>23</v>
-      </c>
-      <c r="O54" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>25</v>
-      </c>
-      <c r="R54" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="12.75">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
         <v>318</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>319</v>
-      </c>
-      <c r="C55" t="s">
-        <v>191</v>
       </c>
       <c r="D55" t="s">
         <v>16</v>
@@ -5025,22 +5578,22 @@
         <v>320</v>
       </c>
       <c r="H55" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I55" t="s">
         <v>321</v>
       </c>
       <c r="J55" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K55" t="s">
         <v>23</v>
       </c>
       <c r="L55" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="M55" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="N55" t="s">
         <v>23</v>
@@ -5058,7 +5611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="12.75">
+    <row r="56" spans="1:18">
       <c r="A56" t="s">
         <v>322</v>
       </c>
@@ -5075,19 +5628,19 @@
         <v>17</v>
       </c>
       <c r="F56" t="s">
-        <v>18</v>
+        <v>325</v>
       </c>
       <c r="G56" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H56" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I56" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J56" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K56" t="s">
         <v>23</v>
@@ -5096,7 +5649,7 @@
         <v>23</v>
       </c>
       <c r="M56" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="N56" t="s">
         <v>23</v>
@@ -5105,7 +5658,7 @@
         <v>23</v>
       </c>
       <c r="P56" t="s">
-        <v>23</v>
+        <v>328</v>
       </c>
       <c r="Q56" t="s">
         <v>25</v>
@@ -5114,15 +5667,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="12.75">
+    <row r="57" spans="1:18">
       <c r="A57" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B57" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C57" t="s">
-        <v>329</v>
+        <v>202</v>
       </c>
       <c r="D57" t="s">
         <v>16</v>
@@ -5131,25 +5684,25 @@
         <v>17</v>
       </c>
       <c r="F57" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G57" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H57" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I57" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J57" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K57" t="s">
         <v>23</v>
       </c>
       <c r="L57" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M57" t="s">
         <v>23</v>
@@ -5161,7 +5714,7 @@
         <v>23</v>
       </c>
       <c r="P57" t="s">
-        <v>333</v>
+        <v>23</v>
       </c>
       <c r="Q57" t="s">
         <v>25</v>
@@ -5170,7 +5723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="12.75">
+    <row r="58" spans="1:18">
       <c r="A58" t="s">
         <v>334</v>
       </c>
@@ -5178,7 +5731,7 @@
         <v>335</v>
       </c>
       <c r="C58" t="s">
-        <v>202</v>
+        <v>336</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
@@ -5187,25 +5740,25 @@
         <v>17</v>
       </c>
       <c r="F58" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G58" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H58" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="I58" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J58" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K58" t="s">
         <v>23</v>
       </c>
       <c r="L58" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="M58" t="s">
         <v>23</v>
@@ -5217,7 +5770,7 @@
         <v>23</v>
       </c>
       <c r="P58" t="s">
-        <v>23</v>
+        <v>340</v>
       </c>
       <c r="Q58" t="s">
         <v>25</v>
@@ -5226,15 +5779,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="12.75">
+    <row r="59" spans="1:18">
       <c r="A59" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B59" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C59" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D59" t="s">
         <v>16</v>
@@ -5243,19 +5796,19 @@
         <v>17</v>
       </c>
       <c r="F59" t="s">
-        <v>342</v>
+        <v>18</v>
       </c>
       <c r="G59" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I59" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J59" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K59" t="s">
         <v>23</v>
@@ -5264,7 +5817,7 @@
         <v>23</v>
       </c>
       <c r="M59" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="N59" t="s">
         <v>23</v>
@@ -5273,7 +5826,7 @@
         <v>23</v>
       </c>
       <c r="P59" t="s">
-        <v>345</v>
+        <v>23</v>
       </c>
       <c r="Q59" t="s">
         <v>25</v>
@@ -5282,7 +5835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="12.75">
+    <row r="60" spans="1:18">
       <c r="A60" t="s">
         <v>346</v>
       </c>
@@ -5299,28 +5852,28 @@
         <v>17</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>349</v>
       </c>
       <c r="G60" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H60" t="s">
         <v>30</v>
       </c>
       <c r="I60" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J60" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="K60" t="s">
         <v>23</v>
       </c>
       <c r="L60" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M60" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="N60" t="s">
         <v>23</v>
@@ -5338,15 +5891,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="12.75">
+    <row r="61" spans="1:18">
       <c r="A61" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C61" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D61" t="s">
         <v>16</v>
@@ -5355,16 +5908,16 @@
         <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G61" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H61" t="s">
-        <v>30</v>
+        <v>209</v>
       </c>
       <c r="I61" t="s">
-        <v>356</v>
+        <v>23</v>
       </c>
       <c r="J61" t="s">
         <v>13</v>
@@ -5394,7 +5947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="12.75">
+    <row r="62" spans="1:18">
       <c r="A62" t="s">
         <v>357</v>
       </c>
@@ -5411,28 +5964,28 @@
         <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="G62" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="H62" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="I62" t="s">
-        <v>23</v>
+        <v>362</v>
       </c>
       <c r="J62" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K62" t="s">
         <v>23</v>
       </c>
       <c r="L62" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M62" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="N62" t="s">
         <v>23</v>
@@ -5450,15 +6003,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="12.75">
+    <row r="63" spans="1:18">
       <c r="A63" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B63" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C63" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D63" t="s">
         <v>16</v>
@@ -5467,318 +6020,318 @@
         <v>17</v>
       </c>
       <c r="F63" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="G63" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="H63" t="s">
         <v>20</v>
       </c>
       <c r="I63" t="s">
+        <v>368</v>
+      </c>
+      <c r="J63" t="s">
+        <v>22</v>
+      </c>
+      <c r="K63" t="s">
+        <v>23</v>
+      </c>
+      <c r="L63" t="s">
+        <v>23</v>
+      </c>
+      <c r="M63" t="s">
+        <v>23</v>
+      </c>
+      <c r="N63" t="s">
+        <v>23</v>
+      </c>
+      <c r="O63" t="s">
+        <v>23</v>
+      </c>
+      <c r="P63" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>25</v>
+      </c>
+      <c r="R63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="A64" t="s">
+        <v>370</v>
+      </c>
+      <c r="B64" t="s">
+        <v>371</v>
+      </c>
+      <c r="C64" t="s">
+        <v>372</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s">
+        <v>373</v>
+      </c>
+      <c r="G64" t="s">
+        <v>374</v>
+      </c>
+      <c r="H64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I64" t="s">
+        <v>375</v>
+      </c>
+      <c r="J64" t="s">
+        <v>13</v>
+      </c>
+      <c r="K64" t="s">
+        <v>23</v>
+      </c>
+      <c r="L64" t="s">
+        <v>45</v>
+      </c>
+      <c r="M64" t="s">
+        <v>23</v>
+      </c>
+      <c r="N64" t="s">
+        <v>23</v>
+      </c>
+      <c r="O64" t="s">
+        <v>23</v>
+      </c>
+      <c r="P64" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>25</v>
+      </c>
+      <c r="R64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" t="s">
+        <v>376</v>
+      </c>
+      <c r="B65" t="s">
+        <v>377</v>
+      </c>
+      <c r="C65" t="s">
+        <v>378</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>379</v>
+      </c>
+      <c r="G65" t="s">
+        <v>380</v>
+      </c>
+      <c r="H65" t="s">
+        <v>289</v>
+      </c>
+      <c r="I65" t="s">
+        <v>381</v>
+      </c>
+      <c r="J65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" t="s">
+        <v>23</v>
+      </c>
+      <c r="L65" t="s">
+        <v>23</v>
+      </c>
+      <c r="M65" t="s">
+        <v>23</v>
+      </c>
+      <c r="N65" t="s">
+        <v>23</v>
+      </c>
+      <c r="O65" t="s">
+        <v>23</v>
+      </c>
+      <c r="P65" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>25</v>
+      </c>
+      <c r="R65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="A66" t="s">
+        <v>382</v>
+      </c>
+      <c r="B66" t="s">
+        <v>383</v>
+      </c>
+      <c r="C66" t="s">
+        <v>230</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>384</v>
+      </c>
+      <c r="G66" t="s">
+        <v>385</v>
+      </c>
+      <c r="H66" t="s">
+        <v>37</v>
+      </c>
+      <c r="I66" t="s">
+        <v>386</v>
+      </c>
+      <c r="J66" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M66" t="s">
+        <v>23</v>
+      </c>
+      <c r="N66" t="s">
+        <v>23</v>
+      </c>
+      <c r="O66" t="s">
+        <v>23</v>
+      </c>
+      <c r="P66" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>387</v>
+      </c>
+      <c r="R66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="A67" t="s">
+        <v>388</v>
+      </c>
+      <c r="B67" t="s">
+        <v>389</v>
+      </c>
+      <c r="C67" t="s">
         <v>365</v>
       </c>
-      <c r="J63" t="s">
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>390</v>
+      </c>
+      <c r="G67" t="s">
+        <v>391</v>
+      </c>
+      <c r="H67" t="s">
+        <v>30</v>
+      </c>
+      <c r="I67" t="s">
+        <v>392</v>
+      </c>
+      <c r="J67" t="s">
         <v>26</v>
       </c>
-      <c r="K63" t="s">
-        <v>23</v>
-      </c>
-      <c r="L63" t="s">
-        <v>23</v>
-      </c>
-      <c r="M63" t="s">
-        <v>56</v>
-      </c>
-      <c r="N63" t="s">
-        <v>23</v>
-      </c>
-      <c r="O63" t="s">
-        <v>23</v>
-      </c>
-      <c r="P63" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>25</v>
-      </c>
-      <c r="R63" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="12.75">
-      <c r="A64" t="s">
-        <v>366</v>
-      </c>
-      <c r="B64" t="s">
-        <v>367</v>
-      </c>
-      <c r="C64" t="s">
-        <v>368</v>
-      </c>
-      <c r="D64" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s">
-        <v>369</v>
-      </c>
-      <c r="G64" t="s">
-        <v>370</v>
-      </c>
-      <c r="H64" t="s">
+      <c r="K67" t="s">
+        <v>23</v>
+      </c>
+      <c r="L67" t="s">
+        <v>23</v>
+      </c>
+      <c r="M67" t="s">
+        <v>79</v>
+      </c>
+      <c r="N67" t="s">
+        <v>23</v>
+      </c>
+      <c r="O67" t="s">
+        <v>23</v>
+      </c>
+      <c r="P67" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>25</v>
+      </c>
+      <c r="R67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" t="s">
+        <v>393</v>
+      </c>
+      <c r="B68" t="s">
+        <v>394</v>
+      </c>
+      <c r="C68" t="s">
+        <v>395</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>396</v>
+      </c>
+      <c r="G68" t="s">
+        <v>397</v>
+      </c>
+      <c r="H68" t="s">
         <v>20</v>
       </c>
-      <c r="I64" t="s">
-        <v>371</v>
-      </c>
-      <c r="J64" t="s">
+      <c r="I68" t="s">
+        <v>398</v>
+      </c>
+      <c r="J68" t="s">
         <v>22</v>
       </c>
-      <c r="K64" t="s">
-        <v>23</v>
-      </c>
-      <c r="L64" t="s">
-        <v>23</v>
-      </c>
-      <c r="M64" t="s">
-        <v>23</v>
-      </c>
-      <c r="N64" t="s">
-        <v>23</v>
-      </c>
-      <c r="O64" t="s">
-        <v>23</v>
-      </c>
-      <c r="P64" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>25</v>
-      </c>
-      <c r="R64" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="12.75">
-      <c r="A65" t="s">
-        <v>373</v>
-      </c>
-      <c r="B65" t="s">
-        <v>374</v>
-      </c>
-      <c r="C65" t="s">
-        <v>375</v>
-      </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" t="s">
-        <v>17</v>
-      </c>
-      <c r="F65" t="s">
-        <v>376</v>
-      </c>
-      <c r="G65" t="s">
-        <v>377</v>
-      </c>
-      <c r="H65" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" t="s">
-        <v>378</v>
-      </c>
-      <c r="J65" t="s">
-        <v>13</v>
-      </c>
-      <c r="K65" t="s">
-        <v>23</v>
-      </c>
-      <c r="L65" t="s">
+      <c r="K68" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68" t="s">
+        <v>23</v>
+      </c>
+      <c r="N68" t="s">
+        <v>23</v>
+      </c>
+      <c r="O68" t="s">
+        <v>23</v>
+      </c>
+      <c r="P68" t="s">
         <v>45</v>
       </c>
-      <c r="M65" t="s">
-        <v>23</v>
-      </c>
-      <c r="N65" t="s">
-        <v>23</v>
-      </c>
-      <c r="O65" t="s">
-        <v>23</v>
-      </c>
-      <c r="P65" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>25</v>
-      </c>
-      <c r="R65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="12.75">
-      <c r="A66" t="s">
-        <v>379</v>
-      </c>
-      <c r="B66" t="s">
-        <v>380</v>
-      </c>
-      <c r="C66" t="s">
-        <v>381</v>
-      </c>
-      <c r="D66" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" t="s">
-        <v>382</v>
-      </c>
-      <c r="G66" t="s">
-        <v>383</v>
-      </c>
-      <c r="H66" t="s">
-        <v>289</v>
-      </c>
-      <c r="I66" t="s">
-        <v>384</v>
-      </c>
-      <c r="J66" t="s">
-        <v>22</v>
-      </c>
-      <c r="K66" t="s">
-        <v>23</v>
-      </c>
-      <c r="L66" t="s">
-        <v>23</v>
-      </c>
-      <c r="M66" t="s">
-        <v>23</v>
-      </c>
-      <c r="N66" t="s">
-        <v>23</v>
-      </c>
-      <c r="O66" t="s">
-        <v>23</v>
-      </c>
-      <c r="P66" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>25</v>
-      </c>
-      <c r="R66" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="12.75">
-      <c r="A67" t="s">
-        <v>385</v>
-      </c>
-      <c r="B67" t="s">
-        <v>386</v>
-      </c>
-      <c r="C67" t="s">
-        <v>230</v>
-      </c>
-      <c r="D67" t="s">
-        <v>16</v>
-      </c>
-      <c r="E67" t="s">
-        <v>17</v>
-      </c>
-      <c r="F67" t="s">
-        <v>387</v>
-      </c>
-      <c r="G67" t="s">
-        <v>388</v>
-      </c>
-      <c r="H67" t="s">
-        <v>37</v>
-      </c>
-      <c r="I67" t="s">
-        <v>389</v>
-      </c>
-      <c r="J67" t="s">
-        <v>13</v>
-      </c>
-      <c r="K67" t="s">
-        <v>23</v>
-      </c>
-      <c r="L67" t="s">
-        <v>56</v>
-      </c>
-      <c r="M67" t="s">
-        <v>23</v>
-      </c>
-      <c r="N67" t="s">
-        <v>23</v>
-      </c>
-      <c r="O67" t="s">
-        <v>23</v>
-      </c>
-      <c r="P67" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>390</v>
-      </c>
-      <c r="R67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="12.75">
-      <c r="A68" t="s">
-        <v>391</v>
-      </c>
-      <c r="B68" t="s">
-        <v>392</v>
-      </c>
-      <c r="C68" t="s">
-        <v>368</v>
-      </c>
-      <c r="D68" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" t="s">
-        <v>17</v>
-      </c>
-      <c r="F68" t="s">
-        <v>393</v>
-      </c>
-      <c r="G68" t="s">
-        <v>394</v>
-      </c>
-      <c r="H68" t="s">
-        <v>30</v>
-      </c>
-      <c r="I68" t="s">
-        <v>395</v>
-      </c>
-      <c r="J68" t="s">
-        <v>26</v>
-      </c>
-      <c r="K68" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" t="s">
-        <v>23</v>
-      </c>
-      <c r="M68" t="s">
-        <v>79</v>
-      </c>
-      <c r="N68" t="s">
-        <v>23</v>
-      </c>
-      <c r="O68" t="s">
-        <v>23</v>
-      </c>
-      <c r="P68" t="s">
-        <v>23</v>
-      </c>
       <c r="Q68" t="s">
         <v>25</v>
       </c>
@@ -5786,15 +6339,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="12.75">
+    <row r="69" spans="1:18">
       <c r="A69" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B69" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C69" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="D69" t="s">
         <v>16</v>
@@ -5803,19 +6356,19 @@
         <v>17</v>
       </c>
       <c r="F69" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="G69" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H69" t="s">
         <v>20</v>
       </c>
       <c r="I69" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="J69" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K69" t="s">
         <v>23</v>
@@ -5824,7 +6377,7 @@
         <v>23</v>
       </c>
       <c r="M69" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="N69" t="s">
         <v>23</v>
@@ -5833,7 +6386,7 @@
         <v>23</v>
       </c>
       <c r="P69" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="Q69" t="s">
         <v>25</v>
@@ -5842,15 +6395,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="12.75">
+    <row r="70" spans="1:18">
       <c r="A70" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B70" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C70" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D70" t="s">
         <v>16</v>
@@ -5859,28 +6412,28 @@
         <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="G70" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="H70" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I70" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="J70" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="K70" t="s">
         <v>23</v>
       </c>
       <c r="L70" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="M70" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="N70" t="s">
         <v>23</v>
@@ -5898,15 +6451,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="12.75">
+    <row r="71" spans="1:18">
       <c r="A71" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B71" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C71" t="s">
-        <v>410</v>
+        <v>310</v>
       </c>
       <c r="D71" t="s">
         <v>16</v>
@@ -5915,16 +6468,16 @@
         <v>17</v>
       </c>
       <c r="F71" t="s">
-        <v>411</v>
+        <v>18</v>
       </c>
       <c r="G71" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H71" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I71" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="J71" t="s">
         <v>13</v>
@@ -5933,7 +6486,7 @@
         <v>23</v>
       </c>
       <c r="L71" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="M71" t="s">
         <v>23</v>
@@ -5954,15 +6507,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="12.75">
+    <row r="72" spans="1:18">
       <c r="A72" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B72" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C72" t="s">
-        <v>310</v>
+        <v>417</v>
       </c>
       <c r="D72" t="s">
         <v>16</v>
@@ -5974,13 +6527,13 @@
         <v>18</v>
       </c>
       <c r="G72" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="H72" t="s">
         <v>37</v>
       </c>
       <c r="I72" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="J72" t="s">
         <v>13</v>
@@ -5989,7 +6542,7 @@
         <v>23</v>
       </c>
       <c r="L72" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="M72" t="s">
         <v>23</v>
@@ -6010,15 +6563,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="12.75">
+    <row r="73" spans="1:18">
       <c r="A73" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B73" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C73" t="s">
-        <v>420</v>
+        <v>343</v>
       </c>
       <c r="D73" t="s">
         <v>16</v>
@@ -6027,28 +6580,28 @@
         <v>17</v>
       </c>
       <c r="F73" t="s">
-        <v>18</v>
+        <v>422</v>
       </c>
       <c r="G73" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="H73" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I73" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J73" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K73" t="s">
         <v>23</v>
       </c>
       <c r="L73" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="M73" t="s">
-        <v>23</v>
+        <v>425</v>
       </c>
       <c r="N73" t="s">
         <v>23</v>
@@ -6060,21 +6613,21 @@
         <v>23</v>
       </c>
       <c r="Q73" t="s">
-        <v>25</v>
+        <v>423</v>
       </c>
       <c r="R73" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" ht="12.75">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B74" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C74" t="s">
-        <v>348</v>
+        <v>295</v>
       </c>
       <c r="D74" t="s">
         <v>16</v>
@@ -6083,16 +6636,16 @@
         <v>17</v>
       </c>
       <c r="F74" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="G74" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="H74" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I74" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="J74" t="s">
         <v>26</v>
@@ -6104,7 +6657,7 @@
         <v>23</v>
       </c>
       <c r="M74" t="s">
-        <v>317</v>
+        <v>45</v>
       </c>
       <c r="N74" t="s">
         <v>23</v>
@@ -6116,21 +6669,21 @@
         <v>23</v>
       </c>
       <c r="Q74" t="s">
-        <v>426</v>
+        <v>25</v>
       </c>
       <c r="R74" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" ht="12.75">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B75" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C75" t="s">
-        <v>295</v>
+        <v>433</v>
       </c>
       <c r="D75" t="s">
         <v>16</v>
@@ -6139,16 +6692,16 @@
         <v>17</v>
       </c>
       <c r="F75" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="G75" t="s">
-        <v>431</v>
+        <v>260</v>
       </c>
       <c r="H75" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I75" t="s">
-        <v>432</v>
+        <v>261</v>
       </c>
       <c r="J75" t="s">
         <v>26</v>
@@ -6160,234 +6713,234 @@
         <v>23</v>
       </c>
       <c r="M75" t="s">
+        <v>98</v>
+      </c>
+      <c r="N75" t="s">
+        <v>23</v>
+      </c>
+      <c r="O75" t="s">
+        <v>23</v>
+      </c>
+      <c r="P75" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>258</v>
+      </c>
+      <c r="R75" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="A76" t="s">
+        <v>435</v>
+      </c>
+      <c r="B76" t="s">
+        <v>436</v>
+      </c>
+      <c r="C76" t="s">
+        <v>129</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F76" t="s">
+        <v>18</v>
+      </c>
+      <c r="G76" t="s">
+        <v>437</v>
+      </c>
+      <c r="H76" t="s">
+        <v>289</v>
+      </c>
+      <c r="I76" t="s">
+        <v>438</v>
+      </c>
+      <c r="J76" t="s">
+        <v>22</v>
+      </c>
+      <c r="K76" t="s">
+        <v>23</v>
+      </c>
+      <c r="L76" t="s">
+        <v>23</v>
+      </c>
+      <c r="M76" t="s">
+        <v>23</v>
+      </c>
+      <c r="N76" t="s">
+        <v>23</v>
+      </c>
+      <c r="O76" t="s">
+        <v>23</v>
+      </c>
+      <c r="P76" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>439</v>
+      </c>
+      <c r="R76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
+      <c r="A77" t="s">
+        <v>440</v>
+      </c>
+      <c r="B77" t="s">
+        <v>441</v>
+      </c>
+      <c r="C77" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F77" t="s">
+        <v>442</v>
+      </c>
+      <c r="G77" t="s">
+        <v>443</v>
+      </c>
+      <c r="H77" t="s">
+        <v>444</v>
+      </c>
+      <c r="I77" t="s">
+        <v>445</v>
+      </c>
+      <c r="J77" t="s">
+        <v>13</v>
+      </c>
+      <c r="K77" t="s">
+        <v>23</v>
+      </c>
+      <c r="L77" t="s">
+        <v>98</v>
+      </c>
+      <c r="M77" t="s">
+        <v>23</v>
+      </c>
+      <c r="N77" t="s">
+        <v>23</v>
+      </c>
+      <c r="O77" t="s">
+        <v>23</v>
+      </c>
+      <c r="P77" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>25</v>
+      </c>
+      <c r="R77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
+      <c r="A78" t="s">
+        <v>446</v>
+      </c>
+      <c r="B78" t="s">
+        <v>447</v>
+      </c>
+      <c r="C78" t="s">
+        <v>365</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>17</v>
+      </c>
+      <c r="F78" t="s">
+        <v>448</v>
+      </c>
+      <c r="G78" t="s">
+        <v>449</v>
+      </c>
+      <c r="H78" t="s">
+        <v>20</v>
+      </c>
+      <c r="I78" t="s">
+        <v>450</v>
+      </c>
+      <c r="J78" t="s">
+        <v>33</v>
+      </c>
+      <c r="K78" t="s">
+        <v>23</v>
+      </c>
+      <c r="L78" t="s">
+        <v>23</v>
+      </c>
+      <c r="M78" t="s">
+        <v>23</v>
+      </c>
+      <c r="N78" t="s">
         <v>45</v>
       </c>
-      <c r="N75" t="s">
-        <v>23</v>
-      </c>
-      <c r="O75" t="s">
-        <v>23</v>
-      </c>
-      <c r="P75" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>25</v>
-      </c>
-      <c r="R75" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" ht="12.75">
-      <c r="A76" t="s">
-        <v>433</v>
-      </c>
-      <c r="B76" t="s">
-        <v>434</v>
-      </c>
-      <c r="C76" t="s">
-        <v>435</v>
-      </c>
-      <c r="D76" t="s">
-        <v>16</v>
-      </c>
-      <c r="E76" t="s">
-        <v>17</v>
-      </c>
-      <c r="F76" t="s">
-        <v>436</v>
-      </c>
-      <c r="G76" t="s">
-        <v>260</v>
-      </c>
-      <c r="H76" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" t="s">
-        <v>261</v>
-      </c>
-      <c r="J76" t="s">
-        <v>26</v>
-      </c>
-      <c r="K76" t="s">
-        <v>23</v>
-      </c>
-      <c r="L76" t="s">
-        <v>23</v>
-      </c>
-      <c r="M76" t="s">
-        <v>98</v>
-      </c>
-      <c r="N76" t="s">
-        <v>23</v>
-      </c>
-      <c r="O76" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>258</v>
-      </c>
-      <c r="R76" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" ht="12.75">
-      <c r="A77" t="s">
-        <v>437</v>
-      </c>
-      <c r="B77" t="s">
-        <v>438</v>
-      </c>
-      <c r="C77" t="s">
-        <v>129</v>
-      </c>
-      <c r="D77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" t="s">
-        <v>17</v>
-      </c>
-      <c r="F77" t="s">
-        <v>18</v>
-      </c>
-      <c r="G77" t="s">
-        <v>439</v>
-      </c>
-      <c r="H77" t="s">
-        <v>289</v>
-      </c>
-      <c r="I77" t="s">
-        <v>440</v>
-      </c>
-      <c r="J77" t="s">
-        <v>22</v>
-      </c>
-      <c r="K77" t="s">
-        <v>23</v>
-      </c>
-      <c r="L77" t="s">
-        <v>23</v>
-      </c>
-      <c r="M77" t="s">
-        <v>23</v>
-      </c>
-      <c r="N77" t="s">
-        <v>23</v>
-      </c>
-      <c r="O77" t="s">
-        <v>23</v>
-      </c>
-      <c r="P77" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>441</v>
-      </c>
-      <c r="R77" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" ht="12.75">
-      <c r="A78" t="s">
-        <v>442</v>
-      </c>
-      <c r="B78" t="s">
-        <v>443</v>
-      </c>
-      <c r="C78" t="s">
-        <v>235</v>
-      </c>
-      <c r="D78" t="s">
-        <v>16</v>
-      </c>
-      <c r="E78" t="s">
-        <v>17</v>
-      </c>
-      <c r="F78" t="s">
-        <v>444</v>
-      </c>
-      <c r="G78" t="s">
-        <v>445</v>
-      </c>
-      <c r="H78" t="s">
-        <v>446</v>
-      </c>
-      <c r="I78" t="s">
-        <v>447</v>
-      </c>
-      <c r="J78" t="s">
+      <c r="O78" t="s">
+        <v>23</v>
+      </c>
+      <c r="P78" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>25</v>
+      </c>
+      <c r="R78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="A79" t="s">
+        <v>451</v>
+      </c>
+      <c r="B79" t="s">
+        <v>452</v>
+      </c>
+      <c r="C79" t="s">
+        <v>295</v>
+      </c>
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" t="s">
+        <v>17</v>
+      </c>
+      <c r="F79" t="s">
+        <v>453</v>
+      </c>
+      <c r="G79" t="s">
+        <v>454</v>
+      </c>
+      <c r="H79" t="s">
+        <v>37</v>
+      </c>
+      <c r="I79" t="s">
+        <v>455</v>
+      </c>
+      <c r="J79" t="s">
         <v>13</v>
       </c>
-      <c r="K78" t="s">
-        <v>23</v>
-      </c>
-      <c r="L78" t="s">
-        <v>98</v>
-      </c>
-      <c r="M78" t="s">
-        <v>23</v>
-      </c>
-      <c r="N78" t="s">
-        <v>23</v>
-      </c>
-      <c r="O78" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>25</v>
-      </c>
-      <c r="R78" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" ht="12.75">
-      <c r="A79" t="s">
-        <v>448</v>
-      </c>
-      <c r="B79" t="s">
-        <v>449</v>
-      </c>
-      <c r="C79" t="s">
-        <v>368</v>
-      </c>
-      <c r="D79" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" t="s">
-        <v>17</v>
-      </c>
-      <c r="F79" t="s">
-        <v>450</v>
-      </c>
-      <c r="G79" t="s">
-        <v>451</v>
-      </c>
-      <c r="H79" t="s">
-        <v>20</v>
-      </c>
-      <c r="I79" t="s">
-        <v>452</v>
-      </c>
-      <c r="J79" t="s">
-        <v>33</v>
-      </c>
       <c r="K79" t="s">
         <v>23</v>
       </c>
       <c r="L79" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M79" t="s">
         <v>23</v>
       </c>
       <c r="N79" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="O79" t="s">
         <v>23</v>
@@ -6402,15 +6955,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="12.75">
+    <row r="80" spans="1:18">
       <c r="A80" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B80" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C80" t="s">
-        <v>295</v>
+        <v>458</v>
       </c>
       <c r="D80" t="s">
         <v>16</v>
@@ -6419,25 +6972,25 @@
         <v>17</v>
       </c>
       <c r="F80" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="G80" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="H80" t="s">
         <v>37</v>
       </c>
       <c r="I80" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="J80" t="s">
-        <v>13</v>
+        <v>291</v>
       </c>
       <c r="K80" t="s">
-        <v>23</v>
+        <v>292</v>
       </c>
       <c r="L80" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="M80" t="s">
         <v>23</v>
@@ -6458,16 +7011,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="12.75">
+    <row r="81" spans="1:18">
       <c r="A81" t="s">
+        <v>462</v>
+      </c>
+      <c r="B81" t="s">
+        <v>463</v>
+      </c>
+      <c r="C81" t="s">
         <v>458</v>
       </c>
-      <c r="B81" t="s">
-        <v>459</v>
-      </c>
-      <c r="C81" t="s">
-        <v>460</v>
-      </c>
       <c r="D81" t="s">
         <v>16</v>
       </c>
@@ -6475,16 +7028,16 @@
         <v>17</v>
       </c>
       <c r="F81" t="s">
-        <v>461</v>
+        <v>18</v>
       </c>
       <c r="G81" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H81" t="s">
-        <v>37</v>
+        <v>289</v>
       </c>
       <c r="I81" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="J81" t="s">
         <v>291</v>
@@ -6514,15 +7067,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="12.75">
+    <row r="82" spans="1:18">
       <c r="A82" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B82" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C82" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="D82" t="s">
         <v>16</v>
@@ -6531,22 +7084,22 @@
         <v>17</v>
       </c>
       <c r="F82" t="s">
-        <v>18</v>
+        <v>469</v>
       </c>
       <c r="G82" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="H82" t="s">
         <v>289</v>
       </c>
       <c r="I82" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="J82" t="s">
-        <v>291</v>
+        <v>22</v>
       </c>
       <c r="K82" t="s">
-        <v>292</v>
+        <v>23</v>
       </c>
       <c r="L82" t="s">
         <v>23</v>
@@ -6561,7 +7114,7 @@
         <v>23</v>
       </c>
       <c r="P82" t="s">
-        <v>23</v>
+        <v>340</v>
       </c>
       <c r="Q82" t="s">
         <v>25</v>
@@ -6570,15 +7123,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="12.75">
+    <row r="83" spans="1:18">
       <c r="A83" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B83" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C83" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="D83" t="s">
         <v>16</v>
@@ -6587,19 +7140,19 @@
         <v>17</v>
       </c>
       <c r="F83" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="G83" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="H83" t="s">
-        <v>289</v>
+        <v>30</v>
       </c>
       <c r="I83" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="J83" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K83" t="s">
         <v>23</v>
@@ -6608,7 +7161,7 @@
         <v>23</v>
       </c>
       <c r="M83" t="s">
-        <v>23</v>
+        <v>478</v>
       </c>
       <c r="N83" t="s">
         <v>23</v>
@@ -6617,7 +7170,7 @@
         <v>23</v>
       </c>
       <c r="P83" t="s">
-        <v>345</v>
+        <v>23</v>
       </c>
       <c r="Q83" t="s">
         <v>25</v>
@@ -6626,15 +7179,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="12.75">
+    <row r="84" spans="1:18">
       <c r="A84" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B84" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C84" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="D84" t="s">
         <v>16</v>
@@ -6643,28 +7196,28 @@
         <v>17</v>
       </c>
       <c r="F84" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="G84" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="H84" t="s">
-        <v>30</v>
+        <v>444</v>
       </c>
       <c r="I84" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="J84" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="K84" t="s">
         <v>23</v>
       </c>
       <c r="L84" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="M84" t="s">
-        <v>480</v>
+        <v>23</v>
       </c>
       <c r="N84" t="s">
         <v>23</v>
@@ -6682,15 +7235,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="12.75">
+    <row r="85" spans="1:18">
       <c r="A85" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B85" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C85" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D85" t="s">
         <v>16</v>
@@ -6699,16 +7252,16 @@
         <v>17</v>
       </c>
       <c r="F85" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="G85" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="H85" t="s">
-        <v>446</v>
+        <v>37</v>
       </c>
       <c r="I85" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="J85" t="s">
         <v>13</v>
@@ -6717,7 +7270,7 @@
         <v>23</v>
       </c>
       <c r="L85" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="M85" t="s">
         <v>23</v>
@@ -6735,67 +7288,12 @@
         <v>25</v>
       </c>
       <c r="R85" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" ht="12.75">
-      <c r="A86" t="s">
-        <v>487</v>
-      </c>
-      <c r="B86" t="s">
-        <v>488</v>
-      </c>
-      <c r="C86" t="s">
-        <v>489</v>
-      </c>
-      <c r="D86" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" t="s">
-        <v>17</v>
-      </c>
-      <c r="F86" t="s">
-        <v>490</v>
-      </c>
-      <c r="G86" t="s">
-        <v>491</v>
-      </c>
-      <c r="H86" t="s">
-        <v>37</v>
-      </c>
-      <c r="I86" t="s">
-        <v>492</v>
-      </c>
-      <c r="J86" t="s">
-        <v>13</v>
-      </c>
-      <c r="K86" t="s">
-        <v>23</v>
-      </c>
-      <c r="L86" t="s">
-        <v>98</v>
-      </c>
-      <c r="M86" t="s">
-        <v>23</v>
-      </c>
-      <c r="N86" t="s">
-        <v>23</v>
-      </c>
-      <c r="O86" t="s">
-        <v>23</v>
-      </c>
-      <c r="P86" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>25</v>
-      </c>
-      <c r="R86" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>